<commit_message>
Analyse & Ontwerp  & Planning document
</commit_message>
<xml_diff>
--- a/______________Rep/Planning.xlsx
+++ b/______________Rep/Planning.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="17">
   <si>
     <t>Uit te voeren activiteit</t>
   </si>
@@ -60,6 +60,21 @@
   </si>
   <si>
     <t>Dag</t>
+  </si>
+  <si>
+    <t>Gemaakte klassendiagram implementeren</t>
+  </si>
+  <si>
+    <t>PLSQL SP's maken</t>
+  </si>
+  <si>
+    <t>PLSQL implementeren in ASP.NET</t>
+  </si>
+  <si>
+    <t>Code  implementeren</t>
+  </si>
+  <si>
+    <t>Testen</t>
   </si>
 </sst>
 </file>
@@ -95,7 +110,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -227,13 +242,22 @@
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
@@ -249,6 +273,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -529,7 +556,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -608,10 +635,13 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="14">
-        <v>42183</v>
+        <v>42185</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
@@ -619,32 +649,117 @@
       <c r="B8" s="9" t="s">
         <v>9</v>
       </c>
+      <c r="C8" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="8"/>
       <c r="B9" s="9" t="s">
         <v>10</v>
       </c>
+      <c r="C9" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="8"/>
-      <c r="B10" s="9"/>
+      <c r="A10" s="14">
+        <v>42186</v>
+      </c>
+      <c r="B10" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C10" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="8"/>
-      <c r="B11" s="9"/>
+      <c r="B11" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="8"/>
-      <c r="B12" s="9"/>
+      <c r="B12" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="8"/>
-      <c r="B13" s="9"/>
+      <c r="A13" s="14">
+        <v>42187</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C13" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="8"/>
-      <c r="B14" s="9"/>
+      <c r="B14" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" s="8"/>
+      <c r="B15" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="14">
+        <v>42188</v>
+      </c>
+      <c r="B16" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="C16" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="17"/>
+      <c r="E16" s="17"/>
+      <c r="F16" s="17"/>
+      <c r="G16" s="17"/>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" s="8"/>
+      <c r="B17" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="B18" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="C18" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" s="16"/>
+      <c r="B19" s="16"/>
+      <c r="C19" s="16"/>
+      <c r="D19" s="16"/>
+      <c r="E19" s="16"/>
+      <c r="F19" s="16"/>
+      <c r="G19" s="16"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
1e Fase Feedback verwerkt
</commit_message>
<xml_diff>
--- a/______________Rep/Planning.xlsx
+++ b/______________Rep/Planning.xlsx
@@ -635,7 +635,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="14">
-        <v>42185</v>
+        <v>42184</v>
       </c>
       <c r="B7" s="9" t="s">
         <v>8</v>
@@ -664,7 +664,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="14">
-        <v>42186</v>
+        <v>42185</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>8</v>
@@ -693,7 +693,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="14">
-        <v>42187</v>
+        <v>42186</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>8</v>
@@ -722,7 +722,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="14">
-        <v>42188</v>
+        <v>42187</v>
       </c>
       <c r="B16" s="9" t="s">
         <v>8</v>

</xml_diff>